<commit_message>
Modifications dans la base de données matériaux
</commit_message>
<xml_diff>
--- a/docs/base de donnees materiaux/BdD materiaux.xlsx
+++ b/docs/base de donnees materiaux/BdD materiaux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clement/Workspace/cpoc-at-omc/docs/base de donnees materiaux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9B7322-B381-1748-9729-36A04DD26617}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F90580-A56C-9149-97B1-6EB98C6540F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,9 @@
     <sheet name="Fonte" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_FilterDatabase" localSheetId="1" hidden="1">Aciers!$R$1:$AA$24</definedName>
+    <definedName name="_FilterDatabase" localSheetId="1" hidden="1">Aciers!$R$1:$Z$24</definedName>
     <definedName name="_FilterDatabase" localSheetId="2" hidden="1">Alu!$R$1:$AA$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Aciers!$R$1:$AA$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Aciers!$R$1:$Z$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alu!$R$1:$AA$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Fonte!$R$1:$AA$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Inox!$R$1:$AA$9</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="262">
   <si>
     <t>Matériau</t>
   </si>
@@ -819,6 +819,15 @@
   </si>
   <si>
     <t>85 I</t>
+  </si>
+  <si>
+    <t>3 : non soudable</t>
+  </si>
+  <si>
+    <t>2 : soudable avec préchauffage</t>
+  </si>
+  <si>
+    <t>1 : facilement soudable</t>
   </si>
 </sst>
 </file>
@@ -1832,13 +1841,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471F9ECE-8D5C-814E-98CE-0956327B3220}">
-  <dimension ref="B1:AB24"/>
+  <dimension ref="B1:Z28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1846,18 +1855,17 @@
     <col min="1" max="17" width="10.83203125" style="1"/>
     <col min="18" max="18" width="98.83203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" style="1" customWidth="1"/>
     <col min="22" max="22" width="19.5" style="1" customWidth="1"/>
     <col min="23" max="23" width="9.5" style="1" customWidth="1"/>
     <col min="24" max="24" width="13.5" style="1" customWidth="1"/>
     <col min="25" max="25" width="13.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="8.5" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.33203125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.83203125" style="1"/>
+    <col min="26" max="26" width="14.83203125" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" s="9" customFormat="1" ht="30">
+    <row r="1" spans="2:26" s="9" customFormat="1" ht="30">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1923,12 +1931,8 @@
       <c r="Z1" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="AA1" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="AB1" s="7"/>
-    </row>
-    <row r="2" spans="2:28" ht="30">
+    </row>
+    <row r="2" spans="2:26" ht="30">
       <c r="B2" s="1" t="s">
         <v>114</v>
       </c>
@@ -1963,10 +1967,10 @@
         <v>1</v>
       </c>
       <c r="Z2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:28" ht="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" ht="30">
       <c r="B3" s="1" t="s">
         <v>117</v>
       </c>
@@ -1997,8 +2001,11 @@
       <c r="U3" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:28" ht="30">
+      <c r="Z3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" ht="30">
       <c r="B4" s="1" t="s">
         <v>120</v>
       </c>
@@ -2011,6 +2018,9 @@
       <c r="J4" s="1">
         <v>510</v>
       </c>
+      <c r="K4" s="1">
+        <v>169</v>
+      </c>
       <c r="L4" s="1">
         <v>6</v>
       </c>
@@ -2036,10 +2046,10 @@
         <v>1</v>
       </c>
       <c r="Z4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26">
       <c r="B5" s="1" t="s">
         <v>123</v>
       </c>
@@ -2052,6 +2062,9 @@
       <c r="J5" s="1">
         <v>490</v>
       </c>
+      <c r="K5" s="1">
+        <v>169</v>
+      </c>
       <c r="L5" s="1">
         <v>7</v>
       </c>
@@ -2074,10 +2087,10 @@
         <v>4</v>
       </c>
       <c r="Z5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26">
       <c r="B6" s="3" t="s">
         <v>126</v>
       </c>
@@ -2115,10 +2128,10 @@
         <v>5</v>
       </c>
       <c r="Z6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26">
       <c r="B7" s="4" t="s">
         <v>130</v>
       </c>
@@ -2159,10 +2172,10 @@
         <v>5</v>
       </c>
       <c r="Z7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26">
       <c r="B8" s="1" t="s">
         <v>134</v>
       </c>
@@ -2197,10 +2210,10 @@
         <v>2</v>
       </c>
       <c r="Z8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26">
       <c r="B9" s="1" t="s">
         <v>137</v>
       </c>
@@ -2231,8 +2244,11 @@
       <c r="V9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:28" ht="45">
+      <c r="Z9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" ht="45">
       <c r="B10" s="1" t="s">
         <v>141</v>
       </c>
@@ -2264,10 +2280,10 @@
         <v>1</v>
       </c>
       <c r="Z10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26">
       <c r="B11" s="1" t="s">
         <v>144</v>
       </c>
@@ -2296,7 +2312,7 @@
         <v>145</v>
       </c>
       <c r="S11" s="1">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="U11" s="1">
         <v>4</v>
@@ -2305,10 +2321,10 @@
         <v>1</v>
       </c>
       <c r="Z11" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" ht="45">
       <c r="B12" s="1" t="s">
         <v>148</v>
       </c>
@@ -2334,7 +2350,7 @@
         <v>150</v>
       </c>
       <c r="S12" s="1">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="U12" s="1">
         <v>2</v>
@@ -2343,10 +2359,10 @@
         <v>1</v>
       </c>
       <c r="Z12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:28" ht="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" ht="30">
       <c r="B13" s="1" t="s">
         <v>151</v>
       </c>
@@ -2377,8 +2393,11 @@
       <c r="V13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:28" ht="30">
+      <c r="Z13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" ht="30">
       <c r="B14" s="1" t="s">
         <v>154</v>
       </c>
@@ -2419,10 +2438,10 @@
         <v>2</v>
       </c>
       <c r="Z14" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:28" ht="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" ht="30">
       <c r="B15" s="1" t="s">
         <v>158</v>
       </c>
@@ -2460,10 +2479,10 @@
         <v>2</v>
       </c>
       <c r="Z15" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" ht="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" ht="30">
       <c r="B16" s="1" t="s">
         <v>162</v>
       </c>
@@ -2501,7 +2520,7 @@
         <v>2</v>
       </c>
       <c r="Z16" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:26" ht="30">
@@ -2530,7 +2549,7 @@
         <v>167</v>
       </c>
       <c r="S17" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="T17" s="1">
         <v>1</v>
@@ -2545,7 +2564,7 @@
         <v>2</v>
       </c>
       <c r="Z17" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:26" ht="30">
@@ -2589,7 +2608,7 @@
         <v>4</v>
       </c>
       <c r="Z18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:26" ht="30">
@@ -2629,6 +2648,9 @@
       <c r="Y19" s="1">
         <v>2</v>
       </c>
+      <c r="Z19" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="2:26" ht="30">
       <c r="B20" s="1" t="s">
@@ -2662,7 +2684,7 @@
         <v>3</v>
       </c>
       <c r="Z20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:26" ht="30">
@@ -2703,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="Z21" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:26">
@@ -2741,7 +2763,7 @@
         <v>1</v>
       </c>
       <c r="Z22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:26" ht="45">
@@ -2773,7 +2795,7 @@
         <v>196</v>
       </c>
       <c r="S23" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U23" s="1">
         <v>2</v>
@@ -2782,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="Z23" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:26" ht="45">
@@ -2823,11 +2845,26 @@
         <v>1</v>
       </c>
       <c r="Z24" s="1">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:26">
+      <c r="Z26" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="2:26">
+      <c r="Z27" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="28" spans="2:26">
+      <c r="Z28" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="R1:AA24" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <autoFilter ref="R1:Z24" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="4" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modifications valeurs définissant les propriétés des matériaux
</commit_message>
<xml_diff>
--- a/docs/base de donnees materiaux/BdD materiaux.xlsx
+++ b/docs/base de donnees materiaux/BdD materiaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clement/Workspace/cpoc-at-omc/docs/base de donnees materiaux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F90580-A56C-9149-97B1-6EB98C6540F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1351821-A3C3-764A-B729-4553D64C1B07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Aciers!$R$1:$Z$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alu!$R$1:$AA$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Fonte!$R$1:$AA$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Inox!$R$1:$AA$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Laiton!$R$1:$AA$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Inox!$R$1:$Z$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Laiton!$R$1:$Z$3</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="262">
   <si>
     <t>Matériau</t>
   </si>
@@ -569,9 +569,6 @@
     <t>AlMgSi0,5</t>
   </si>
   <si>
-    <t>bien Anodisable, ben aspect. Bonne tenue à la corrosion, très bien soudable, mauvaise fragmebtabilité du copeau et mauvaise capacité d'emboutissage.  Mal usinable</t>
-  </si>
-  <si>
     <t>6262 A</t>
   </si>
   <si>
@@ -828,6 +825,9 @@
   </si>
   <si>
     <t>1 : facilement soudable</t>
+  </si>
+  <si>
+    <t>bien Anodisable, bel aspect. Bonne tenue à la corrosion, très bien soudable, mauvaise fragmebtabilité du copeau et mauvaise capacité d'emboutissage.  Mal usinable</t>
   </si>
 </sst>
 </file>
@@ -1843,11 +1843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471F9ECE-8D5C-814E-98CE-0956327B3220}">
   <dimension ref="B1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1911,25 +1911,25 @@
         <v>36</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="2" spans="2:26" ht="30">
@@ -2010,7 +2010,7 @@
         <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I4" s="1">
         <v>440</v>
@@ -2054,7 +2054,7 @@
         <v>123</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I5" s="1">
         <v>410</v>
@@ -2235,6 +2235,9 @@
       <c r="N9" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="P9" s="1">
+        <v>936</v>
+      </c>
       <c r="R9" s="2" t="s">
         <v>140</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>171</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I19" s="1">
         <v>900</v>
@@ -2654,7 +2657,7 @@
     </row>
     <row r="20" spans="2:26" ht="30">
       <c r="B20" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>51</v>
@@ -2675,7 +2678,7 @@
         <v>1022</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S20" s="1">
         <v>60</v>
@@ -2689,10 +2692,10 @@
     </row>
     <row r="21" spans="2:26" ht="30">
       <c r="B21" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I21" s="1">
         <v>300</v>
@@ -2707,13 +2710,13 @@
         <v>18</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P21" s="1">
         <v>785</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S21" s="1">
         <v>50</v>
@@ -2730,10 +2733,10 @@
     </row>
     <row r="22" spans="2:26">
       <c r="B22" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="I22" s="1">
         <v>260</v>
@@ -2751,7 +2754,7 @@
         <v>978</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S22" s="1">
         <v>47</v>
@@ -2768,10 +2771,10 @@
     </row>
     <row r="23" spans="2:26" ht="45">
       <c r="B23" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="G23" s="1">
         <v>210</v>
@@ -2792,7 +2795,7 @@
         <v>785</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="S23" s="1">
         <v>100</v>
@@ -2809,7 +2812,7 @@
     </row>
     <row r="24" spans="2:26" ht="45">
       <c r="B24" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G24" s="1">
         <v>200</v>
@@ -2827,13 +2830,13 @@
         <v>10</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P24" s="1">
         <v>800</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S24" s="1">
         <v>41</v>
@@ -2850,17 +2853,17 @@
     </row>
     <row r="26" spans="2:26">
       <c r="Z26" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="2:26">
       <c r="Z27" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="2:26">
       <c r="Z28" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2878,7 +2881,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R26" sqref="R26"/>
+      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2943,33 +2946,33 @@
         <v>36</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="2" spans="2:27" ht="30">
       <c r="B2" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>146</v>
@@ -2978,10 +2981,10 @@
         <v>74</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="L2" s="1">
         <v>10</v>
@@ -3007,7 +3010,7 @@
     </row>
     <row r="3" spans="2:27" ht="30">
       <c r="B3" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>146</v>
@@ -3060,10 +3063,10 @@
         <v>8</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>175</v>
+        <v>261</v>
       </c>
       <c r="S4" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="T4" s="1">
         <v>4</v>
@@ -3077,10 +3080,10 @@
     </row>
     <row r="5" spans="2:27">
       <c r="B5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="G5" s="1">
         <v>68.3</v>
@@ -3104,7 +3107,7 @@
         <v>3610</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S5" s="1">
         <v>100</v>
@@ -3112,10 +3115,10 @@
     </row>
     <row r="6" spans="2:27" ht="30">
       <c r="B6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="G6" s="1">
         <v>76</v>
@@ -3133,10 +3136,10 @@
         <v>0.5</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S6" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="V6" s="1">
         <v>4</v>
@@ -3147,7 +3150,7 @@
     </row>
     <row r="7" spans="2:27" ht="30">
       <c r="B7" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G7" s="1">
         <v>70</v>
@@ -3168,7 +3171,10 @@
         <v>8</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="S7" s="1">
+        <v>110</v>
       </c>
       <c r="T7" s="1">
         <v>1</v>
@@ -3185,7 +3191,7 @@
     </row>
     <row r="8" spans="2:27" ht="30">
       <c r="B8" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F8" s="1">
         <v>2.71</v>
@@ -3209,10 +3215,10 @@
         <v>4</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S8" s="1">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="X8" s="1">
         <v>4</v>
@@ -3223,10 +3229,10 @@
     </row>
     <row r="9" spans="2:27" ht="30">
       <c r="B9" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="G9" s="1">
         <v>69.099999999999994</v>
@@ -3244,10 +3250,10 @@
         <v>10</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S9" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U9" s="1">
         <v>2</v>
@@ -3267,10 +3273,10 @@
     </row>
     <row r="10" spans="2:27" ht="30">
       <c r="B10" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="G10" s="1">
         <v>69.5</v>
@@ -3291,10 +3297,10 @@
         <v>8</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="S10" s="1">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="X10" s="1">
         <v>2</v>
@@ -3315,13 +3321,597 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50E0626-187A-8641-B3DB-E474EE2CB96A}">
-  <dimension ref="B1:AA9"/>
+  <dimension ref="B1:Z9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="17" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="98.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" ht="30">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="2:26" ht="30">
+      <c r="B2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G2" s="1">
+        <v>185</v>
+      </c>
+      <c r="I2" s="1">
+        <v>190</v>
+      </c>
+      <c r="J2" s="1">
+        <v>500</v>
+      </c>
+      <c r="K2" s="1">
+        <v>330</v>
+      </c>
+      <c r="L2" s="1">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1">
+        <v>3700</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="S2" s="1">
+        <v>65</v>
+      </c>
+      <c r="U2" s="1">
+        <v>3</v>
+      </c>
+      <c r="W2" s="1">
+        <v>5</v>
+      </c>
+      <c r="X2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" ht="30">
+      <c r="B3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="I3" s="1">
+        <v>597</v>
+      </c>
+      <c r="J3" s="1">
+        <v>750</v>
+      </c>
+      <c r="K3" s="1">
+        <v>245</v>
+      </c>
+      <c r="L3" s="1">
+        <v>9</v>
+      </c>
+      <c r="P3" s="1">
+        <v>2065</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="S3" s="1">
+        <v>58</v>
+      </c>
+      <c r="U3" s="1">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" ht="30">
+      <c r="B4" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="1">
+        <v>201</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I4" s="1">
+        <v>175</v>
+      </c>
+      <c r="J4" s="1">
+        <v>500</v>
+      </c>
+      <c r="K4" s="1">
+        <v>220</v>
+      </c>
+      <c r="L4" s="1">
+        <v>35</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1580</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="S4" s="1">
+        <v>45</v>
+      </c>
+      <c r="U4" s="1">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>2</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" ht="30">
+      <c r="B5" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I5" s="1">
+        <v>190</v>
+      </c>
+      <c r="J5" s="1">
+        <v>490</v>
+      </c>
+      <c r="K5" s="1">
+        <v>215</v>
+      </c>
+      <c r="L5" s="1">
+        <v>30</v>
+      </c>
+      <c r="P5" s="1">
+        <v>4600</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="S5" s="1">
+        <v>40</v>
+      </c>
+      <c r="U5" s="1">
+        <v>2</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" ht="30">
+      <c r="B6" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" s="1">
+        <v>220</v>
+      </c>
+      <c r="I6" s="1">
+        <v>200</v>
+      </c>
+      <c r="J6" s="1">
+        <v>420</v>
+      </c>
+      <c r="K6" s="1">
+        <v>180</v>
+      </c>
+      <c r="L6" s="1">
+        <v>20</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2165</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S6" s="1">
+        <v>35</v>
+      </c>
+      <c r="T6" s="1">
+        <v>2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>3</v>
+      </c>
+      <c r="X6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" ht="30">
+      <c r="B7" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="1">
+        <v>650</v>
+      </c>
+      <c r="J7" s="1">
+        <v>780</v>
+      </c>
+      <c r="K7" s="1">
+        <v>245</v>
+      </c>
+      <c r="L7" s="1">
+        <v>10</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1970</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="S7" s="1">
+        <v>45</v>
+      </c>
+      <c r="U7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" ht="30">
+      <c r="B8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="1">
+        <v>316</v>
+      </c>
+      <c r="I8" s="1">
+        <v>190</v>
+      </c>
+      <c r="J8" s="1">
+        <v>500</v>
+      </c>
+      <c r="K8" s="1">
+        <v>315</v>
+      </c>
+      <c r="L8" s="1">
+        <v>20</v>
+      </c>
+      <c r="P8" s="1">
+        <v>2500</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="S8" s="1">
+        <v>40</v>
+      </c>
+      <c r="U8" s="1">
+        <v>2</v>
+      </c>
+      <c r="W8" s="1">
+        <v>2</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26">
+      <c r="B9" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="1">
+        <v>250</v>
+      </c>
+      <c r="J9" s="1">
+        <v>430</v>
+      </c>
+      <c r="K9" s="1">
+        <v>200</v>
+      </c>
+      <c r="L9" s="1">
+        <v>20</v>
+      </c>
+      <c r="P9" s="1">
+        <v>2321</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="S9" s="1">
+        <v>75</v>
+      </c>
+      <c r="X9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="R1:Z9" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4206F29C-4F84-7F41-8FCB-E66AB4EA5704}">
+  <dimension ref="B1:Z3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="17" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="98.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" ht="30">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="2:26" ht="30">
+      <c r="B2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="1">
+        <v>93</v>
+      </c>
+      <c r="I2" s="1">
+        <v>200</v>
+      </c>
+      <c r="J2" s="1">
+        <v>520</v>
+      </c>
+      <c r="K2" s="1">
+        <v>170</v>
+      </c>
+      <c r="L2" s="1">
+        <v>18</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2780</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="X2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" ht="30">
+      <c r="B3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I3" s="1">
+        <v>390</v>
+      </c>
+      <c r="J3" s="1">
+        <v>430</v>
+      </c>
+      <c r="K3" s="1">
+        <v>150</v>
+      </c>
+      <c r="L3" s="1">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="T3" s="1">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="R1:Z3" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9501DF-A527-824C-8F49-AB0BE52A7B29}">
+  <dimension ref="B1:AA4"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3386,663 +3976,77 @@
         <v>36</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="AA1" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="2:27" ht="30">
+    </row>
+    <row r="2" spans="2:27">
       <c r="B2" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="G2" s="1">
-        <v>185</v>
+        <v>170</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.27500000000000002</v>
       </c>
       <c r="I2" s="1">
-        <v>190</v>
+        <v>310</v>
       </c>
       <c r="J2" s="1">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="K2" s="1">
-        <v>330</v>
+        <v>210</v>
       </c>
       <c r="L2" s="1">
-        <v>12</v>
-      </c>
-      <c r="P2" s="1">
-        <v>3700</v>
+        <v>10</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="S2" s="1">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="U2" s="1">
-        <v>3</v>
-      </c>
-      <c r="W2" s="1">
-        <v>5</v>
-      </c>
-      <c r="X2" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:27" ht="30">
-      <c r="B3" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="I3" s="1">
-        <v>597</v>
-      </c>
-      <c r="J3" s="1">
-        <v>750</v>
-      </c>
-      <c r="K3" s="1">
-        <v>245</v>
-      </c>
-      <c r="L3" s="1">
-        <v>9</v>
-      </c>
-      <c r="P3" s="1">
-        <v>2065</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="S3" s="1">
-        <v>58</v>
-      </c>
-      <c r="U3" s="1">
-        <v>2</v>
-      </c>
-      <c r="X3" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:27" ht="30">
-      <c r="B4" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="G4" s="1">
-        <v>201</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I4" s="1">
-        <v>175</v>
-      </c>
-      <c r="J4" s="1">
-        <v>500</v>
-      </c>
-      <c r="K4" s="1">
-        <v>220</v>
-      </c>
-      <c r="L4" s="1">
-        <v>35</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1580</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="S4" s="1">
-        <v>45</v>
-      </c>
-      <c r="U4" s="1">
-        <v>2</v>
-      </c>
-      <c r="W4" s="1">
-        <v>2</v>
-      </c>
-      <c r="X4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:27" ht="30">
-      <c r="B5" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I5" s="1">
-        <v>190</v>
-      </c>
-      <c r="J5" s="1">
-        <v>490</v>
-      </c>
-      <c r="K5" s="1">
-        <v>215</v>
-      </c>
-      <c r="L5" s="1">
-        <v>30</v>
-      </c>
-      <c r="P5" s="1">
-        <v>4600</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="S5" s="1">
-        <v>40</v>
-      </c>
-      <c r="U5" s="1">
-        <v>2</v>
-      </c>
-      <c r="X5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:27" ht="30">
-      <c r="B6" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G6" s="1">
-        <v>220</v>
-      </c>
-      <c r="I6" s="1">
-        <v>200</v>
-      </c>
-      <c r="J6" s="1">
-        <v>420</v>
-      </c>
-      <c r="K6" s="1">
-        <v>180</v>
-      </c>
-      <c r="L6" s="1">
-        <v>20</v>
-      </c>
-      <c r="P6" s="1">
-        <v>2165</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="S6" s="1">
-        <v>35</v>
-      </c>
-      <c r="T6" s="1">
-        <v>2</v>
-      </c>
-      <c r="W6" s="1">
-        <v>3</v>
-      </c>
-      <c r="X6" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:27" ht="30">
-      <c r="B7" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="1">
-        <v>650</v>
-      </c>
-      <c r="J7" s="1">
-        <v>780</v>
-      </c>
-      <c r="K7" s="1">
-        <v>245</v>
-      </c>
-      <c r="L7" s="1">
-        <v>10</v>
-      </c>
-      <c r="P7" s="1">
-        <v>1970</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="S7" s="1">
-        <v>45</v>
-      </c>
-      <c r="U7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:27" ht="30">
-      <c r="B8" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C8" s="1">
-        <v>316</v>
-      </c>
-      <c r="I8" s="1">
-        <v>190</v>
-      </c>
-      <c r="J8" s="1">
-        <v>500</v>
-      </c>
-      <c r="K8" s="1">
-        <v>315</v>
-      </c>
-      <c r="L8" s="1">
-        <v>20</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="S8" s="1">
-        <v>40</v>
-      </c>
-      <c r="U8" s="1">
-        <v>2</v>
-      </c>
-      <c r="W8" s="1">
-        <v>2</v>
-      </c>
-      <c r="X8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:27">
-      <c r="B9" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I9" s="1">
-        <v>250</v>
-      </c>
-      <c r="J9" s="1">
-        <v>430</v>
-      </c>
-      <c r="K9" s="1">
-        <v>200</v>
-      </c>
-      <c r="L9" s="1">
-        <v>20</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="S9" s="1">
-        <v>75</v>
-      </c>
-      <c r="X9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="R1:AA9" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4206F29C-4F84-7F41-8FCB-E66AB4EA5704}">
-  <dimension ref="B1:AA3"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB1" sqref="AB1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="17" width="10.83203125" style="1"/>
-    <col min="18" max="18" width="98.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="8.5" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.33203125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:27" ht="30">
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="2:27" ht="30">
-      <c r="B2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" s="1">
-        <v>93</v>
-      </c>
-      <c r="I2" s="1">
-        <v>200</v>
-      </c>
-      <c r="J2" s="1">
-        <v>520</v>
-      </c>
-      <c r="K2" s="1">
-        <v>170</v>
-      </c>
-      <c r="L2" s="1">
-        <v>18</v>
-      </c>
-      <c r="P2" s="1">
-        <v>2780</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="X2" s="1">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>4</v>
       </c>
       <c r="Z2" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:27" ht="30">
-      <c r="B3" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I3" s="1">
-        <v>390</v>
-      </c>
-      <c r="J3" s="1">
-        <v>430</v>
-      </c>
-      <c r="K3" s="1">
-        <v>150</v>
-      </c>
-      <c r="L3" s="1">
-        <v>8</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="T3" s="1">
-        <v>2</v>
-      </c>
-      <c r="X3" s="1">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="R1:AA3" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9501DF-A527-824C-8F49-AB0BE52A7B29}">
-  <dimension ref="B1:AA4"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="17" width="10.83203125" style="1"/>
-    <col min="18" max="18" width="98.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="8.5" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.33203125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:27" ht="30">
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="2:27">
-      <c r="B2" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" s="1">
-        <v>170</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="I2" s="1">
-        <v>310</v>
-      </c>
-      <c r="J2" s="1">
-        <v>450</v>
-      </c>
-      <c r="K2" s="1">
-        <v>210</v>
-      </c>
-      <c r="L2" s="1">
-        <v>10</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="S2" s="1">
-        <v>3</v>
-      </c>
-      <c r="U2" s="1">
-        <v>4</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>4</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>4</v>
-      </c>
-    </row>
     <row r="3" spans="2:27">
       <c r="B3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="G3" s="1">
         <v>103</v>
@@ -4063,10 +4067,10 @@
         <v>0.3</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="U3" s="1">
         <v>5</v>
@@ -4080,10 +4084,10 @@
     </row>
     <row r="4" spans="2:27">
       <c r="B4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="G4" s="1">
         <v>103</v>
@@ -4104,10 +4108,10 @@
         <v>0.3</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S4" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="U4" s="1">
         <v>5</v>

</xml_diff>

<commit_message>
Mise à jour des paramètres matériaux
</commit_message>
<xml_diff>
--- a/docs/base de donnees materiaux/BdD materiaux.xlsx
+++ b/docs/base de donnees materiaux/BdD materiaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clement/Workspace/cpoc-at-omc/docs/base de donnees materiaux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1351821-A3C3-764A-B729-4553D64C1B07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0920EFF-8F06-0C48-B35B-617348E3FE3E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1843,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471F9ECE-8D5C-814E-98CE-0956327B3220}">
   <dimension ref="B1:Z28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
@@ -3731,7 +3731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4206F29C-4F84-7F41-8FCB-E66AB4EA5704}">
   <dimension ref="B1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Ajout fichier BdD suite à une erreur
</commit_message>
<xml_diff>
--- a/docs/base de donnees materiaux/BdD materiaux.xlsx
+++ b/docs/base de donnees materiaux/BdD materiaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clement/Workspace/cpoc-at-omc/docs/base de donnees materiaux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0920EFF-8F06-0C48-B35B-617348E3FE3E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1351821-A3C3-764A-B729-4553D64C1B07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1843,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471F9ECE-8D5C-814E-98CE-0956327B3220}">
   <dimension ref="B1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
@@ -3731,7 +3731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4206F29C-4F84-7F41-8FCB-E66AB4EA5704}">
   <dimension ref="B1:Z3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Ajout js et correction anglais dans les interfaces
</commit_message>
<xml_diff>
--- a/docs/base de donnees materiaux/BdD materiaux.xlsx
+++ b/docs/base de donnees materiaux/BdD materiaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clement/Workspace/cpoc-at-omc/docs/base de donnees materiaux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1351821-A3C3-764A-B729-4553D64C1B07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915B7208-7D4E-DC44-B9D9-E88B44AC6B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13880" yWindow="460" windowWidth="10000" windowHeight="14560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1843,11 +1843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471F9ECE-8D5C-814E-98CE-0956327B3220}">
   <dimension ref="B1:Z28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2875,13 +2875,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084ADA29-3FC8-704E-AEA5-3C9B0E480466}">
-  <dimension ref="B1:AA10"/>
+  <dimension ref="B1:AA11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3310,6 +3310,11 @@
       </c>
       <c r="AA10" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27">
+      <c r="B11" s="1">
+        <v>6082</v>
       </c>
     </row>
   </sheetData>
@@ -3731,7 +3736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4206F29C-4F84-7F41-8FCB-E66AB4EA5704}">
   <dimension ref="B1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>